<commit_message>
test change in excel
</commit_message>
<xml_diff>
--- a/excels/boston/boston.xlsx
+++ b/excels/boston/boston.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="13260" windowHeight="5010" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="13260" windowHeight="5010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="housing" localSheetId="0">data!$A$1:$D$490</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>RM</t>
   </si>
@@ -56,6 +57,9 @@
   </si>
   <si>
     <t>MEDV</t>
+  </si>
+  <si>
+    <t>added new data to test git</t>
   </si>
 </sst>
 </file>
@@ -3113,11 +3117,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134011520"/>
-        <c:axId val="134009216"/>
+        <c:axId val="118444800"/>
+        <c:axId val="118446720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134011520"/>
+        <c:axId val="118444800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3133,12 +3137,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134009216"/>
+        <c:crossAx val="118446720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134009216"/>
+        <c:axId val="118446720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3154,7 +3158,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134011520"/>
+        <c:crossAx val="118444800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10389,8 +10393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B490"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14323,4 +14327,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>